<commit_message>
Upgrading OCV-SOC P25 data
</commit_message>
<xml_diff>
--- a/data/Lab2_data/OCV_SOC_+25.xlsx
+++ b/data/Lab2_data/OCV_SOC_+25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Lab_2\Modle\Project_Lab2\Lab_2\data\Lab2_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEF1B45-185B-452F-AC84-AF8671E5610F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477C1115-9E3F-4A5F-8CA2-07A16616DFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="380" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.7</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.1249799999999999</c:v>
@@ -1297,7 +1297,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="C2">
         <v>3.0914999999999999</v>

</xml_diff>